<commit_message>
Adapt querySting and hash on force reload pages.
</commit_message>
<xml_diff>
--- a/meta/objects/MenuItem.xlsx
+++ b/meta/objects/MenuItem.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A24719C-A2BA-864D-927F-2FD982776409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A248C90F-A674-B84A-89E8-D90026C7E5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29240" yWindow="5720" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25680" yWindow="5720" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="86">
   <si>
     <t>クラス名</t>
   </si>
@@ -522,6 +522,28 @@
   </si>
   <si>
     <t>%</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>queryAndHash</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>RouteQueryAndHash</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>遷移先URLに付加するqueryとhash</t>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">センイサキ </t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">フカスル </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>import { RouteQueryAndHash } from "vue-router"</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1244,27 +1266,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1273,22 +1294,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1298,21 +1318,15 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1324,8 +1338,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1358,45 +1372,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1406,7 +1417,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1415,7 +1426,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1434,25 +1445,25 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1872,10 +1883,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1920,10 +1931,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
+      <c r="G5" s="67"/>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="3" t="s">
@@ -1936,11 +1944,7 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="37"/>
+      <c r="G6" s="68"/>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="3" t="s">
@@ -1950,14 +1954,10 @@
       <c r="C7" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="37"/>
+      <c r="G7" s="68"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="3" t="s">
@@ -1965,33 +1965,25 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="10"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="37"/>
+      <c r="G8" s="68"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="98" t="s">
+      <c r="A9" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="99"/>
+      <c r="B9" s="88"/>
       <c r="C9" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="79" t="s">
+      <c r="G9" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="37"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="3" t="s">
@@ -1999,33 +1991,26 @@
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="10"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="37"/>
+      <c r="G10" s="68"/>
     </row>
     <row r="11" spans="1:13" ht="29" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="100" t="s">
+      <c r="C11" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="101"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="3" t="s">
@@ -2038,69 +2023,63 @@
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-    </row>
-    <row r="13" spans="1:13" s="31" customFormat="1">
-      <c r="A13" s="64" t="s">
+      <c r="G12" s="68"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="65"/>
-      <c r="C13" s="66" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="57" t="s">
         <v>54</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="71"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
       <c r="K13"/>
     </row>
-    <row r="14" spans="1:13" s="31" customFormat="1">
-      <c r="A14" s="64" t="s">
+    <row r="14" spans="1:13">
+      <c r="A14" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="65"/>
-      <c r="C14" s="66"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="57"/>
       <c r="D14" t="s">
         <v>47</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="71"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
       <c r="K14"/>
     </row>
-    <row r="15" spans="1:13" s="31" customFormat="1">
-      <c r="A15" s="64" t="s">
+    <row r="15" spans="1:13">
+      <c r="A15" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="65"/>
-      <c r="C15" s="66"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="57"/>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
-      <c r="H15" s="68"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="71"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:13" s="31" customFormat="1">
-      <c r="A16" s="110" t="s">
+    <row r="16" spans="1:13">
+      <c r="A16" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="111"/>
-      <c r="C16" s="66" t="s">
+      <c r="B16" s="100"/>
+      <c r="C16" s="57" t="s">
         <v>32</v>
       </c>
       <c r="D16" t="s">
@@ -2109,64 +2088,64 @@
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="71"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
       <c r="K16"/>
     </row>
-    <row r="17" spans="1:15" s="31" customFormat="1">
-      <c r="A17" s="64" t="s">
+    <row r="17" spans="1:14">
+      <c r="A17" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="65"/>
-      <c r="C17" s="66"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="57"/>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="71"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
       <c r="K17"/>
     </row>
-    <row r="18" spans="1:15" s="31" customFormat="1">
-      <c r="A18" s="64" t="s">
+    <row r="18" spans="1:14">
+      <c r="A18" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="65"/>
-      <c r="C18" s="66"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="57"/>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="71"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
       <c r="K18"/>
     </row>
-    <row r="19" spans="1:15" s="31" customFormat="1">
-      <c r="A19" s="64" t="s">
+    <row r="19" spans="1:14">
+      <c r="A19" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="65"/>
-      <c r="C19" s="66" t="s">
+      <c r="B19" s="13"/>
+      <c r="C19" s="57" t="s">
         <v>32</v>
       </c>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19"/>
       <c r="G19"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="68"/>
-      <c r="J19" s="71"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
       <c r="K19"/>
     </row>
-    <row r="20" spans="1:15" s="31" customFormat="1">
-      <c r="A20" s="110" t="s">
+    <row r="20" spans="1:14">
+      <c r="A20" s="99" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="111"/>
-      <c r="C20" s="66" t="s">
+      <c r="B20" s="100"/>
+      <c r="C20" s="57" t="s">
         <v>32</v>
       </c>
       <c r="D20" t="s">
@@ -2175,80 +2154,50 @@
       <c r="E20"/>
       <c r="F20"/>
       <c r="G20"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="71"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
       <c r="K20"/>
     </row>
-    <row r="21" spans="1:15" s="39" customFormat="1">
-      <c r="A21" s="36"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-    </row>
-    <row r="22" spans="1:15">
-      <c r="A22" s="29" t="s">
+    <row r="21" spans="1:14">
+      <c r="B21"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
-    </row>
-    <row r="23" spans="1:15">
-      <c r="A23" s="32" t="s">
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="61"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="69"/>
-      <c r="I23" s="69"/>
-      <c r="J23" s="69"/>
-      <c r="K23" s="69"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="31"/>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="B23" s="31"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="59"/>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="10"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="37"/>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="63"/>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="3" t="s">
         <v>14</v>
       </c>
@@ -2256,712 +2205,665 @@
       <c r="C25" s="7"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="37"/>
-    </row>
-    <row r="26" spans="1:15">
-      <c r="A26" s="36"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="37"/>
-    </row>
-    <row r="27" spans="1:15">
-      <c r="A27" s="29" t="s">
+      <c r="F25" s="64"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="B26"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="46"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="46"/>
-      <c r="K27" s="46"/>
-      <c r="L27" s="45"/>
-      <c r="M27" s="45"/>
-      <c r="N27" s="45"/>
-      <c r="O27" s="45"/>
-    </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="49" t="s">
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="69"/>
-      <c r="I28" s="69"/>
-      <c r="J28" s="69"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="46"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="47"/>
-      <c r="O28" s="37"/>
-    </row>
-    <row r="29" spans="1:15">
-      <c r="A29" s="53"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="70"/>
-      <c r="H29" s="70"/>
-      <c r="I29" s="70"/>
-      <c r="J29" s="70"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="38"/>
-      <c r="N29" s="38"/>
-      <c r="O29" s="37"/>
-    </row>
-    <row r="30" spans="1:15">
-      <c r="A30" s="53"/>
-      <c r="B30" s="48"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="70"/>
-      <c r="H30" s="70"/>
-      <c r="I30" s="70"/>
-      <c r="J30" s="70"/>
-      <c r="K30" s="36"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="38"/>
-      <c r="N30" s="38"/>
-      <c r="O30" s="37"/>
-    </row>
-    <row r="31" spans="1:15">
-      <c r="A31" s="54"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="70"/>
-      <c r="H31" s="70"/>
-      <c r="I31" s="70"/>
-      <c r="J31" s="70"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="38"/>
-      <c r="M31" s="38"/>
-      <c r="N31" s="38"/>
-      <c r="O31" s="37"/>
-    </row>
-    <row r="32" spans="1:15" s="39" customFormat="1">
-      <c r="A32" s="36"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="36"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="59"/>
+      <c r="J28" s="59"/>
+      <c r="K28" s="59"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="39"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="45"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="60"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="45"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="46"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="B32"/>
     </row>
     <row r="33" spans="1:15">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="46"/>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="45"/>
-      <c r="M33" s="45"/>
-      <c r="N33" s="45"/>
-      <c r="O33" s="45"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
     </row>
     <row r="34" spans="1:15">
-      <c r="A34" s="49" t="s">
+      <c r="A34" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="69"/>
-      <c r="K34" s="69"/>
-      <c r="L34" s="46"/>
-      <c r="M34" s="47"/>
-      <c r="N34" s="47"/>
-      <c r="O34" s="37"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="59"/>
+      <c r="J34" s="59"/>
+      <c r="K34" s="59"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="39"/>
     </row>
     <row r="35" spans="1:15">
-      <c r="A35" s="53"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="40"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="70"/>
-      <c r="H35" s="70"/>
-      <c r="I35" s="70"/>
-      <c r="J35" s="70"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="38"/>
-      <c r="M35" s="38"/>
-      <c r="N35" s="38"/>
-      <c r="O35" s="37"/>
+      <c r="A35" s="45"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="60"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
     </row>
     <row r="36" spans="1:15">
-      <c r="A36" s="53"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="70"/>
-      <c r="H36" s="70"/>
-      <c r="I36" s="70"/>
-      <c r="J36" s="70"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="38"/>
-      <c r="M36" s="38"/>
-      <c r="N36" s="38"/>
-      <c r="O36" s="37"/>
+      <c r="A36" s="45"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="60"/>
+      <c r="H36" s="60"/>
+      <c r="I36" s="60"/>
+      <c r="J36" s="60"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
     </row>
     <row r="37" spans="1:15">
-      <c r="A37" s="54"/>
-      <c r="B37" s="50"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="70"/>
-      <c r="H37" s="70"/>
-      <c r="I37" s="70"/>
-      <c r="J37" s="70"/>
-      <c r="K37" s="36"/>
-      <c r="L37" s="38"/>
-      <c r="M37" s="38"/>
-      <c r="N37" s="38"/>
-      <c r="O37" s="37"/>
+      <c r="A37" s="46"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="60"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="60"/>
+      <c r="J37" s="60"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
+      <c r="A38"/>
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
     </row>
     <row r="39" spans="1:15">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="46"/>
-      <c r="H39" s="46"/>
-      <c r="I39" s="46"/>
-      <c r="J39" s="46"/>
-      <c r="K39" s="46"/>
-      <c r="L39" s="45"/>
-      <c r="M39" s="45"/>
-      <c r="N39" s="45"/>
-      <c r="O39" s="45"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
     </row>
     <row r="40" spans="1:15">
-      <c r="A40" s="49" t="s">
+      <c r="A40" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="44" t="s">
+      <c r="B40" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="44"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="44"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="69"/>
-      <c r="H40" s="69"/>
-      <c r="I40" s="69"/>
-      <c r="J40" s="69"/>
-      <c r="K40" s="69"/>
-      <c r="L40" s="46"/>
-      <c r="M40" s="47"/>
-      <c r="N40" s="47"/>
-      <c r="O40" s="37"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="59"/>
+      <c r="H40" s="59"/>
+      <c r="I40" s="59"/>
+      <c r="J40" s="59"/>
+      <c r="K40" s="59"/>
+      <c r="M40" s="39"/>
+      <c r="N40" s="39"/>
     </row>
     <row r="41" spans="1:15">
-      <c r="A41" s="53"/>
-      <c r="B41" s="48"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="40"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="70"/>
-      <c r="H41" s="70"/>
-      <c r="I41" s="70"/>
-      <c r="J41" s="70"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="38"/>
-      <c r="M41" s="38"/>
-      <c r="N41" s="38"/>
-      <c r="O41" s="37"/>
+      <c r="A41" s="45">
+        <v>1</v>
+      </c>
+      <c r="B41" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="60"/>
+      <c r="H41" s="60"/>
+      <c r="I41" s="60"/>
+      <c r="J41" s="60"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
     </row>
     <row r="42" spans="1:15">
-      <c r="A42" s="53"/>
-      <c r="B42" s="48"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="70"/>
-      <c r="H42" s="70"/>
-      <c r="I42" s="70"/>
-      <c r="J42" s="70"/>
-      <c r="K42" s="36"/>
-      <c r="L42" s="38"/>
-      <c r="M42" s="38"/>
-      <c r="N42" s="38"/>
-      <c r="O42" s="37"/>
+      <c r="A42" s="45"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="60"/>
+      <c r="H42" s="60"/>
+      <c r="I42" s="60"/>
+      <c r="J42" s="60"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
     </row>
     <row r="43" spans="1:15">
-      <c r="A43" s="54"/>
-      <c r="B43" s="50"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="51"/>
-      <c r="E43" s="51"/>
-      <c r="F43" s="52"/>
-      <c r="G43" s="70"/>
-      <c r="H43" s="70"/>
-      <c r="I43" s="70"/>
-      <c r="J43" s="70"/>
-      <c r="K43" s="36"/>
-      <c r="L43" s="38"/>
-      <c r="M43" s="38"/>
-      <c r="N43" s="38"/>
-      <c r="O43" s="37"/>
+      <c r="A43" s="46"/>
+      <c r="B43" s="42"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="60"/>
+      <c r="H43" s="60"/>
+      <c r="I43" s="60"/>
+      <c r="J43" s="60"/>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
     </row>
     <row r="44" spans="1:15">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13"/>
+      <c r="A44"/>
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
     </row>
     <row r="45" spans="1:15">
       <c r="A45" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
       <c r="N45" s="6"/>
-      <c r="O45" s="15"/>
+      <c r="O45" s="14"/>
     </row>
     <row r="46" spans="1:15" ht="13.5" customHeight="1">
-      <c r="A46" s="104" t="s">
+      <c r="A46" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="B46" s="104" t="s">
+      <c r="B46" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="C46" s="103" t="s">
+      <c r="C46" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="103" t="s">
+      <c r="D46" s="92" t="s">
         <v>13</v>
       </c>
-      <c r="E46" s="105" t="s">
+      <c r="E46" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="F46" s="103" t="s">
+      <c r="F46" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="G46" s="105" t="s">
+      <c r="G46" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="H46" s="105" t="s">
+      <c r="H46" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="I46" s="108" t="s">
+      <c r="I46" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="J46" s="108" t="s">
+      <c r="J46" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="K46" s="103" t="s">
+      <c r="K46" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="L46" s="103"/>
-      <c r="M46" s="16"/>
-      <c r="N46" s="17"/>
+      <c r="L46" s="92"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="16"/>
       <c r="O46" s="9"/>
     </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="104"/>
-      <c r="B47" s="104"/>
-      <c r="C47" s="103"/>
-      <c r="D47" s="103"/>
-      <c r="E47" s="106"/>
-      <c r="F47" s="103"/>
-      <c r="G47" s="107"/>
-      <c r="H47" s="107"/>
-      <c r="I47" s="109"/>
-      <c r="J47" s="109"/>
-      <c r="K47" s="103"/>
-      <c r="L47" s="103"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="28"/>
-      <c r="O47" s="15"/>
+      <c r="A47" s="93"/>
+      <c r="B47" s="93"/>
+      <c r="C47" s="92"/>
+      <c r="D47" s="92"/>
+      <c r="E47" s="95"/>
+      <c r="F47" s="92"/>
+      <c r="G47" s="96"/>
+      <c r="H47" s="96"/>
+      <c r="I47" s="98"/>
+      <c r="J47" s="98"/>
+      <c r="K47" s="92"/>
+      <c r="L47" s="92"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="27"/>
+      <c r="O47" s="14"/>
     </row>
     <row r="48" spans="1:15">
-      <c r="A48" s="19">
+      <c r="A48" s="18">
         <v>1</v>
       </c>
-      <c r="B48" s="81" t="s">
+      <c r="B48" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="88" t="s">
+      <c r="C48" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="76"/>
-      <c r="I48" s="76"/>
-      <c r="J48" s="76"/>
-      <c r="K48" s="20" t="s">
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="65"/>
+      <c r="I48" s="65"/>
+      <c r="J48" s="65"/>
+      <c r="K48" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="L48" s="21"/>
-      <c r="M48" s="21"/>
-      <c r="N48" s="27"/>
-      <c r="O48" s="15"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="20"/>
+      <c r="N48" s="26"/>
+      <c r="O48" s="14"/>
     </row>
     <row r="49" spans="1:15">
-      <c r="A49" s="19">
+      <c r="A49" s="18">
         <f>A48+1</f>
         <v>2</v>
       </c>
-      <c r="B49" s="81" t="s">
+      <c r="B49" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="C49" s="88" t="s">
+      <c r="C49" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="76"/>
-      <c r="I49" s="76"/>
-      <c r="J49" s="76"/>
-      <c r="K49" s="20" t="s">
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="65"/>
+      <c r="I49" s="65"/>
+      <c r="J49" s="65"/>
+      <c r="K49" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="L49" s="21"/>
-      <c r="M49" s="21"/>
-      <c r="N49" s="27"/>
-      <c r="O49" s="15"/>
+      <c r="L49" s="20"/>
+      <c r="M49" s="20"/>
+      <c r="N49" s="26"/>
+      <c r="O49" s="14"/>
     </row>
     <row r="50" spans="1:15">
-      <c r="A50" s="19">
+      <c r="A50" s="18">
         <f t="shared" ref="A50:A55" si="0">A49+1</f>
         <v>3</v>
       </c>
-      <c r="B50" s="82" t="s">
+      <c r="B50" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="89" t="s">
+      <c r="C50" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="91"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="76" t="s">
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="80"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="I50" s="76"/>
-      <c r="J50" s="76"/>
-      <c r="K50" s="20" t="s">
+      <c r="I50" s="65"/>
+      <c r="J50" s="65"/>
+      <c r="K50" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="L50" s="21"/>
-      <c r="M50" s="21"/>
-      <c r="N50" s="22"/>
-      <c r="O50" s="15"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="20"/>
+      <c r="N50" s="21"/>
+      <c r="O50" s="14"/>
     </row>
     <row r="51" spans="1:15">
-      <c r="A51" s="19">
+      <c r="A51" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B51" s="83" t="s">
+      <c r="B51" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="90" t="s">
+      <c r="C51" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="76" t="s">
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="I51" s="76"/>
-      <c r="J51" s="76"/>
-      <c r="K51" s="20" t="s">
+      <c r="I51" s="65"/>
+      <c r="J51" s="65"/>
+      <c r="K51" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="L51" s="21"/>
-      <c r="M51" s="21"/>
-      <c r="N51" s="22"/>
-      <c r="O51" s="15"/>
+      <c r="L51" s="20"/>
+      <c r="M51" s="20"/>
+      <c r="N51" s="21"/>
+      <c r="O51" s="14"/>
     </row>
     <row r="52" spans="1:15">
-      <c r="A52" s="19">
+      <c r="A52" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B52" s="83" t="s">
+      <c r="B52" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="C52" s="90" t="s">
+      <c r="C52" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="76" t="s">
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="I52" s="76"/>
-      <c r="J52" s="76"/>
-      <c r="K52" s="20" t="s">
+      <c r="I52" s="65"/>
+      <c r="J52" s="65"/>
+      <c r="K52" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="L52" s="21"/>
-      <c r="M52" s="21"/>
-      <c r="N52" s="22"/>
-      <c r="O52" s="15"/>
+      <c r="L52" s="20"/>
+      <c r="M52" s="20"/>
+      <c r="N52" s="21"/>
+      <c r="O52" s="14"/>
     </row>
     <row r="53" spans="1:15">
-      <c r="A53" s="19">
+      <c r="A53" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B53" s="83" t="s">
+      <c r="B53" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="C53" s="90" t="s">
+      <c r="C53" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="D53" s="84"/>
-      <c r="E53" s="84"/>
-      <c r="F53" s="84"/>
-      <c r="G53" s="84"/>
-      <c r="H53" s="85" t="s">
+      <c r="D53" s="73"/>
+      <c r="E53" s="73"/>
+      <c r="F53" s="73"/>
+      <c r="G53" s="73"/>
+      <c r="H53" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="I53" s="85"/>
-      <c r="J53" s="85"/>
-      <c r="K53" s="84" t="s">
+      <c r="I53" s="74"/>
+      <c r="J53" s="74"/>
+      <c r="K53" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="L53" s="86"/>
-      <c r="M53" s="86"/>
-      <c r="N53" s="87"/>
-      <c r="O53" s="15"/>
+      <c r="L53" s="75"/>
+      <c r="M53" s="75"/>
+      <c r="N53" s="76"/>
+      <c r="O53" s="14"/>
     </row>
     <row r="54" spans="1:15">
-      <c r="A54" s="19">
+      <c r="A54" s="18">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B54" s="83" t="s">
+      <c r="B54" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="C54" s="90" t="s">
+      <c r="C54" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="D54" s="84" t="s">
+      <c r="D54" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="E54" s="84"/>
-      <c r="F54" s="84"/>
-      <c r="G54" s="84"/>
-      <c r="H54" s="85" t="s">
+      <c r="E54" s="73"/>
+      <c r="F54" s="73"/>
+      <c r="G54" s="73"/>
+      <c r="H54" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="I54" s="85"/>
-      <c r="J54" s="85"/>
-      <c r="K54" s="84" t="s">
+      <c r="I54" s="74"/>
+      <c r="J54" s="74"/>
+      <c r="K54" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="L54" s="86"/>
-      <c r="M54" s="86"/>
-      <c r="N54" s="87"/>
-      <c r="O54" s="15"/>
+      <c r="L54" s="75"/>
+      <c r="M54" s="75"/>
+      <c r="N54" s="76"/>
+      <c r="O54" s="14"/>
     </row>
     <row r="55" spans="1:15">
-      <c r="A55" s="19">
+      <c r="A55" s="18">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B55" s="93" t="s">
+      <c r="B55" s="82" t="s">
         <v>66</v>
       </c>
-      <c r="C55" s="94" t="s">
+      <c r="C55" s="83" t="s">
         <v>65</v>
       </c>
-      <c r="D55" s="84" t="s">
+      <c r="D55" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="E55" s="84"/>
-      <c r="F55" s="84"/>
-      <c r="G55" s="84"/>
-      <c r="H55" s="85" t="s">
+      <c r="E55" s="73"/>
+      <c r="F55" s="73"/>
+      <c r="G55" s="73"/>
+      <c r="H55" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="I55" s="85"/>
-      <c r="J55" s="85"/>
-      <c r="K55" s="84" t="s">
+      <c r="I55" s="74"/>
+      <c r="J55" s="74"/>
+      <c r="K55" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="L55" s="86"/>
-      <c r="M55" s="86"/>
-      <c r="N55" s="87"/>
-      <c r="O55" s="15"/>
+      <c r="L55" s="75"/>
+      <c r="M55" s="75"/>
+      <c r="N55" s="76"/>
+      <c r="O55" s="14"/>
     </row>
     <row r="56" spans="1:15">
-      <c r="A56" s="92">
+      <c r="A56" s="81">
         <v>9</v>
       </c>
-      <c r="B56" s="95" t="s">
+      <c r="B56" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="C56" s="97" t="s">
+      <c r="C56" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="D56" s="84"/>
-      <c r="E56" s="84"/>
-      <c r="F56" s="84"/>
-      <c r="G56" s="84"/>
-      <c r="H56" s="85" t="s">
+      <c r="D56" s="73"/>
+      <c r="E56" s="73"/>
+      <c r="F56" s="73"/>
+      <c r="G56" s="73"/>
+      <c r="H56" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="I56" s="85"/>
-      <c r="J56" s="85"/>
-      <c r="K56" s="84" t="s">
+      <c r="I56" s="74"/>
+      <c r="J56" s="74"/>
+      <c r="K56" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="L56" s="86"/>
-      <c r="M56" s="86"/>
-      <c r="N56" s="87"/>
-      <c r="O56" s="15"/>
+      <c r="L56" s="75"/>
+      <c r="M56" s="75"/>
+      <c r="N56" s="76"/>
+      <c r="O56" s="14"/>
     </row>
     <row r="57" spans="1:15">
-      <c r="A57" s="92">
+      <c r="A57" s="81">
         <v>10</v>
       </c>
-      <c r="B57" s="95" t="s">
+      <c r="B57" s="84" t="s">
         <v>77</v>
       </c>
-      <c r="C57" s="97" t="s">
+      <c r="C57" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="D57" s="84"/>
-      <c r="E57" s="84"/>
-      <c r="F57" s="84" t="b">
+      <c r="D57" s="73"/>
+      <c r="E57" s="73"/>
+      <c r="F57" s="73" t="b">
         <v>1</v>
       </c>
-      <c r="G57" s="84"/>
-      <c r="H57" s="85" t="s">
+      <c r="G57" s="73"/>
+      <c r="H57" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="I57" s="85"/>
-      <c r="J57" s="85"/>
-      <c r="K57" s="84" t="s">
+      <c r="I57" s="74"/>
+      <c r="J57" s="74"/>
+      <c r="K57" s="73" t="s">
         <v>79</v>
       </c>
-      <c r="L57" s="86"/>
-      <c r="M57" s="86"/>
-      <c r="N57" s="87"/>
-      <c r="O57" s="15"/>
+      <c r="L57" s="75"/>
+      <c r="M57" s="75"/>
+      <c r="N57" s="76"/>
+      <c r="O57" s="14"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="23"/>
-      <c r="B58" s="96"/>
-      <c r="C58" s="96"/>
-      <c r="D58" s="24"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="24"/>
-      <c r="H58" s="77"/>
-      <c r="I58" s="77"/>
-      <c r="J58" s="77"/>
-      <c r="K58" s="24"/>
-      <c r="L58" s="25"/>
-      <c r="M58" s="25"/>
-      <c r="N58" s="26"/>
-      <c r="O58" s="15"/>
+      <c r="A58" s="81">
+        <v>11</v>
+      </c>
+      <c r="B58" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="C58" s="86" t="s">
+        <v>83</v>
+      </c>
+      <c r="D58" s="73"/>
+      <c r="E58" s="73"/>
+      <c r="F58" s="73"/>
+      <c r="G58" s="73"/>
+      <c r="H58" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="I58" s="74"/>
+      <c r="J58" s="74"/>
+      <c r="K58" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="L58" s="75"/>
+      <c r="M58" s="75"/>
+      <c r="N58" s="76"/>
+      <c r="O58" s="14"/>
+    </row>
+    <row r="59" spans="1:15">
+      <c r="A59" s="22"/>
+      <c r="B59" s="85"/>
+      <c r="C59" s="85"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
+      <c r="H59" s="66"/>
+      <c r="I59" s="66"/>
+      <c r="J59" s="66"/>
+      <c r="K59" s="23"/>
+      <c r="L59" s="24"/>
+      <c r="M59" s="24"/>
+      <c r="N59" s="25"/>
+      <c r="O59" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -2983,7 +2885,7 @@
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F74:J74" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F75:J75" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2996,7 +2898,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16 G48:G58" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16 G48:G59" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>isAbstract</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17" xr:uid="{00000000-0002-0000-0000-000005000000}">
@@ -3018,7 +2920,7 @@
           <x14:formula1>
             <xm:f>config!$P$4:$P$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H48:J58</xm:sqref>
+          <xm:sqref>H48:J59</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3039,107 +2941,107 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="57" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="57" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="57" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" style="57" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="57" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" style="57" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="57" customWidth="1"/>
-    <col min="10" max="10" width="18.5" style="57" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="57" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" style="57" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" style="57" customWidth="1"/>
-    <col min="14" max="14" width="18.6640625" style="57" bestFit="1" customWidth="1"/>
-    <col min="15" max="260" width="8.83203125" style="57" customWidth="1"/>
-    <col min="261" max="16384" width="10.83203125" style="57"/>
+    <col min="1" max="3" width="8.83203125" style="49" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="49" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" style="49" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="49" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" style="49" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="49" customWidth="1"/>
+    <col min="10" max="10" width="18.5" style="49" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="49" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="49" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="15" max="260" width="8.83203125" style="49" customWidth="1"/>
+    <col min="261" max="16384" width="10.83203125" style="49"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="56" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="56"/>
+      <c r="Q1" s="48"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="F3" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="58" t="s">
+      <c r="H3" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="58" t="s">
+      <c r="J3" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="58" t="s">
+      <c r="L3" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="58" t="s">
+      <c r="N3" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="58" t="s">
+      <c r="P3" s="50" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="B4" s="59"/>
-      <c r="D4" s="62" t="s">
+      <c r="B4" s="51"/>
+      <c r="D4" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="P4" s="60"/>
+      <c r="H4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="P4" s="52"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="H5" s="62" t="s">
+      <c r="D5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="H5" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="62" t="s">
+      <c r="J5" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="62" t="s">
+      <c r="L5" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="N5" s="62" t="s">
+      <c r="N5" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="62" t="s">
+      <c r="P5" s="54" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="B6" s="63"/>
+      <c r="B6" s="55"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>

</xml_diff>